<commit_message>
split ongoing, finished, always
</commit_message>
<xml_diff>
--- a/src/main/sample.xlsx
+++ b/src/main/sample.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sangjin/Desktop/osj/Brave-Recruit-Script/src/main/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76F393D9-EA0E-B94E-8E20-61221DD30BC9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD689940-9635-364A-87B3-51A557F660E2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17860" yWindow="460" windowWidth="20540" windowHeight="19820" xr2:uid="{10EA807B-2356-F443-B855-2D7BA64B90CB}"/>
+    <workbookView xWindow="21500" yWindow="0" windowWidth="16900" windowHeight="21600" xr2:uid="{10EA807B-2356-F443-B855-2D7BA64B90CB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -462,7 +462,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>

</xml_diff>

<commit_message>
Update README.md in try
</commit_message>
<xml_diff>
--- a/src/main/sample.xlsx
+++ b/src/main/sample.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sangjin/Desktop/osj/Brave-Recruit-Script/src/main/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD689940-9635-364A-87B3-51A557F660E2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09417266-4573-0544-A4E7-A1FDA781E63B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="21500" yWindow="0" windowWidth="16900" windowHeight="21600" xr2:uid="{10EA807B-2356-F443-B855-2D7BA64B90CB}"/>
   </bookViews>
@@ -462,7 +462,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>
@@ -499,7 +499,7 @@
         <v>5</v>
       </c>
       <c r="C3" s="2">
-        <v>44277</v>
+        <v>44310</v>
       </c>
     </row>
     <row r="4" spans="1:3">

</xml_diff>